<commit_message>
DLT: foundation till error
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Ravali\Sem 2\CV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CV_Assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC4D2BB-2573-49BB-B3DA-9FB3F133BD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,108 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>[X ,Y , Z]</t>
+    <t>X</t>
   </si>
   <si>
-    <t>[u, v]</t>
+    <t>Y</t>
   </si>
   <si>
-    <t>(0,0,0)</t>
+    <t>Z</t>
   </si>
   <si>
-    <t>(2805 , 1468)</t>
+    <t>x</t>
   </si>
   <si>
-    <t>(1,0,0)</t>
-  </si>
-  <si>
-    <t>(2187 , 1516)</t>
-  </si>
-  <si>
-    <t>(2,0,2)</t>
-  </si>
-  <si>
-    <t>(2337 , 1322)</t>
-  </si>
-  <si>
-    <t>(0,3,3)</t>
-  </si>
-  <si>
-    <t>(1761, 1240)</t>
-  </si>
-  <si>
-    <t>(0,5,3)</t>
-  </si>
-  <si>
-    <t>(1505 , 1376)</t>
-  </si>
-  <si>
-    <t>(2,0,6)</t>
-  </si>
-  <si>
-    <t>(2405 , 713)</t>
-  </si>
-  <si>
-    <t>(9,0,7)</t>
-  </si>
-  <si>
-    <t>(3774 , 950)</t>
-  </si>
-  <si>
-    <t>(5,4,0)</t>
-  </si>
-  <si>
-    <t>(2309 , 2131)</t>
-  </si>
-  <si>
-    <t>(6,6,0)</t>
-  </si>
-  <si>
-    <t>(2227 , ,2456)</t>
-  </si>
-  <si>
-    <t>(9,7,0)</t>
-  </si>
-  <si>
-    <t>(2652 , 2977)</t>
-  </si>
-  <si>
-    <t>(0,6,7)</t>
-  </si>
-  <si>
-    <t>(0,9,3)</t>
-  </si>
-  <si>
-    <t>(1306 ,720)</t>
-  </si>
-  <si>
-    <t>(835 , 1711)</t>
-  </si>
-  <si>
-    <t>(0,9,7)</t>
-  </si>
-  <si>
-    <t>(658 , 902)</t>
-  </si>
-  <si>
-    <t>(1,0,5)</t>
-  </si>
-  <si>
-    <t>(2251 , 826)</t>
-  </si>
-  <si>
-    <t>(0,0,7)</t>
-  </si>
-  <si>
-    <t>(2143 , 434)</t>
+    <t>y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,10 +57,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,7 +68,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -159,14 +76,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,145 +379,204 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>450</v>
+      </c>
+      <c r="E2">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>137</v>
+      </c>
+      <c r="E3">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>288</v>
+      </c>
+      <c r="E4">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>294</v>
+      </c>
+      <c r="E5">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>462</v>
+      </c>
+      <c r="E6">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>115</v>
+      </c>
+      <c r="E7">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>173</v>
+      </c>
+      <c r="E8">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>7.5</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>237</v>
+      </c>
+      <c r="E9">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>12.5</v>
+      </c>
+      <c r="B10">
+        <v>17.5</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>252</v>
+      </c>
+      <c r="E10">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>328</v>
+      </c>
+      <c r="E11">
+        <v>526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refined dataset and code
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CV_Assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC4D2BB-2573-49BB-B3DA-9FB3F133BD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685E7B3E-F775-4F5B-940F-9C9C8D5AFA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -380,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -392,7 +392,7 @@
     <col min="3" max="3" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,7 +409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20</v>
       </c>
@@ -420,13 +420,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>450</v>
+        <v>708</v>
       </c>
       <c r="E2">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>991</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -437,13 +440,16 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>137</v>
+        <v>213</v>
       </c>
       <c r="E3">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>998</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -454,13 +460,16 @@
         <v>20</v>
       </c>
       <c r="D4">
-        <v>288</v>
+        <v>455</v>
       </c>
       <c r="E4">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>597</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>20</v>
       </c>
@@ -471,13 +480,16 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>294</v>
+        <v>464</v>
       </c>
       <c r="E5">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1192</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>20</v>
       </c>
@@ -488,13 +500,16 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>462</v>
+        <v>727</v>
       </c>
       <c r="E6">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>658</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -505,13 +520,16 @@
         <v>20</v>
       </c>
       <c r="D7">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="E7">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>665</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -522,13 +540,16 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <v>173</v>
+        <v>279</v>
       </c>
       <c r="E8">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>810</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -539,13 +560,16 @@
         <v>15</v>
       </c>
       <c r="D9">
-        <v>237</v>
+        <v>373</v>
       </c>
       <c r="E9">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>699</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>12.5</v>
       </c>
@@ -556,13 +580,16 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>252</v>
+        <v>396</v>
       </c>
       <c r="E10">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1082</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -573,10 +600,173 @@
         <v>5</v>
       </c>
       <c r="D11">
-        <v>328</v>
+        <v>516</v>
       </c>
       <c r="E11">
-        <v>526</v>
+        <v>828</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>463</v>
+      </c>
+      <c r="E12">
+        <v>998</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>576</v>
+      </c>
+      <c r="E13">
+        <v>779</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>343</v>
+      </c>
+      <c r="E14">
+        <v>784</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>463</v>
+      </c>
+      <c r="E15">
+        <v>874</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>529</v>
+      </c>
+      <c r="E16">
+        <v>1038</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>642</v>
+      </c>
+      <c r="E17">
+        <v>805</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>829</v>
+      </c>
+      <c r="E18">
+        <v>576</v>
+      </c>
+      <c r="F18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>76</v>
+      </c>
+      <c r="E19">
+        <v>586</v>
+      </c>
+      <c r="F19">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>